<commit_message>
alterado pasta de destino
</commit_message>
<xml_diff>
--- a/dividir.xlsx
+++ b/dividir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prog-1\Documents\PROJETOS\Dividir_videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EE3E12-7143-4746-906F-CF8F4A30969A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3726E4BC-23DC-426D-9BFF-0AB94C2E2EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="4290" windowWidth="11265" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tempo" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>nome_video_entrada</t>
   </si>
@@ -61,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -95,17 +95,17 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -430,12 +430,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -464,37 +464,28 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>1.9351851851851853E-2</v>
       </c>
       <c r="C2" s="2">
-        <v>3.4722222222222224E-4</v>
+        <v>2.0856481481481479E-2</v>
       </c>
       <c r="D2">
         <f>HOUR($B2)*3600+MINUTE($B2)*60+SECOND($B2)</f>
-        <v>0</v>
+        <v>1672</v>
       </c>
       <c r="E2">
         <f>(HOUR($C2)*3600+MINUTE($C2)*60+SECOND($C2))-$D2</f>
-        <v>30</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>6.9444444444444447E-4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.3888888888888889E-3</v>
-      </c>
       <c r="D3">
         <f t="shared" ref="D3:D66" si="0">HOUR($B3)*3600+MINUTE($B3)*60+SECOND($B3)</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E66" si="1">(HOUR($C3)*3600+MINUTE($C3)*60+SECOND($C3))-$D3</f>
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>